<commit_message>
Added avg of lat and lon to comparisons
and changed the calculation of delta to use absolute value
</commit_message>
<xml_diff>
--- a/doc_ex2/Algorithm comparisons/Algo2 BM2 ts1 comparison.xlsx
+++ b/doc_ex2/Algorithm comparisons/Algo2 BM2 ts1 comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olga\Documents\GitHub\Csv_to_Kml_Converter\doc_ex2\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\GitHub\Csv_to_Kml_Converter\doc_ex2\Algorithm comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
   <si>
     <t>Ariel_University</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Average for all rows</t>
+  </si>
+  <si>
+    <t>Average of Lat and Lon</t>
   </si>
 </sst>
 </file>
@@ -145,9 +148,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,8 +196,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +238,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -392,14 +407,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,8 +457,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -759,25 +780,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1655062-209A-4B36-861B-E6DC8C57DFF6}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.421875" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1"/>
+    <col min="19" max="19" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.25" thickBot="1" x14ac:dyDescent="1">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="16" t="s">
         <v>26</v>
       </c>
@@ -800,8 +823,11 @@
       <c r="Q1" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.85">
+      <c r="S1" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -833,27 +859,31 @@
         <v>705.55776831726098</v>
       </c>
       <c r="L2">
-        <f>C2-H2</f>
-        <v>-6.0489556695131341E-5</v>
+        <f>ABS(C2-H2)</f>
+        <v>6.0489556695131341E-5</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M17" si="0">D2-I2</f>
-        <v>-2.8560796459942139E-4</v>
-      </c>
-      <c r="N2" s="4">
-        <f t="shared" ref="N2:N17" si="1">E2-J2</f>
+        <f t="shared" ref="M2:N17" si="0">ABS(D2-I2)</f>
+        <v>2.8560796459942139E-4</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
         <v>2.2128503227650071</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O10" si="2">(L2+M2+N2)/3</f>
-        <v>0.7375014084145709</v>
+        <f t="shared" ref="O2:O10" si="1">(L2+M2+N2)/3</f>
+        <v>0.73773214009543386</v>
       </c>
       <c r="Q2" s="5">
         <f>AVERAGE(O2:O32)</f>
-        <v>0.85621575247477444</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.85">
+        <v>1.0700901382608008</v>
+      </c>
+      <c r="S2" s="20">
+        <f>AVERAGE(L2:L32,M2:M32)</f>
+        <v>1.4237992923728284E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -885,23 +915,23 @@
         <v>698.67501137809904</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L32" si="3">C3-H3</f>
-        <v>-1.3795821800499652E-5</v>
+        <f t="shared" ref="L3:L32" si="2">ABS(C3-H3)</f>
+        <v>1.3795821800499652E-5</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>-1.1615677380660827E-4</v>
-      </c>
-      <c r="N3" s="4">
+        <v>1.1615677380660827E-4</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>4.3639918861630349</v>
+      </c>
+      <c r="O3">
         <f t="shared" si="1"/>
-        <v>-4.3639918861630349</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="2"/>
-        <v>-1.4547072795862139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.85">
+        <v>1.4547072795862139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -933,23 +963,23 @@
         <v>701.97265254911804</v>
       </c>
       <c r="L4">
-        <f t="shared" si="3"/>
-        <v>-8.6913702503466084E-5</v>
+        <f t="shared" si="2"/>
+        <v>8.6913702503466084E-5</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
         <v>3.8043877395921299E-5</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>2.1129335232379844</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="1"/>
-        <v>2.1129335232379844</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="2"/>
-        <v>0.704294884470959</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.85">
+        <v>0.70435282693929457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -981,23 +1011,23 @@
         <v>700.10606350722105</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.3649296879947315E-4</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
         <v>7.5344636499607986E-5</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>5.6961961940099854</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="1"/>
-        <v>5.6961961940099854</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="2"/>
         <v>1.8988026772050948</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1029,23 +1059,23 @@
         <v>704.13682019881696</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.8373753299982809E-4</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
         <v>2.526922965984113E-4</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>3.7045148800350489</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="1"/>
-        <v>3.7045148800350489</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="2"/>
         <v>1.2349837699548825</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1077,23 +1107,23 @@
         <v>703.79135868017795</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8.1230530298626036E-5</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
         <v>1.2890336599014063E-5</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>2.995321744363082</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="1"/>
-        <v>2.995321744363082</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="2"/>
         <v>0.99847195507665987</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1125,23 +1155,23 @@
         <v>692.314993496537</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.3085719790240091E-4</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
         <v>7.6328081298981942E-5</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>5.2690762492879912</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="1"/>
-        <v>5.2690762492879912</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="2"/>
         <v>1.7564278115223975</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1173,23 +1203,23 @@
         <v>700.115762874393</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0964585810313565E-4</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>-1.4111820250661822E-4</v>
-      </c>
-      <c r="N9" s="4">
+        <v>1.4111820250661822E-4</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>4.8820851205190365</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="1"/>
-        <v>4.8820851205190365</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="2"/>
-        <v>1.6273512160582111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.85">
+        <v>1.6274452948598821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1221,23 +1251,23 @@
         <v>703.29084922601999</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.1887039569890021E-4</v>
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>-2.2809895980913097E-6</v>
-      </c>
-      <c r="N10" s="4">
+        <v>2.2809895980913097E-6</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>4.4395465676070671</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="1"/>
-        <v>4.4395465676070671</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="2"/>
-        <v>1.4799210523377226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.85">
+        <v>1.4799225729974548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1269,23 +1299,23 @@
         <v>702.65990884292398</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.1307520200700765E-5</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>-4.5146821896935307E-5</v>
-      </c>
-      <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <v>4.5146821896935307E-5</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
         <v>0.91569615102002899</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O33" si="4">(L11+M11+N11)/3</f>
-        <v>0.30524743723944425</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.85">
+        <f t="shared" ref="O11:O32" si="3">(L11+M11+N11)/3</f>
+        <v>0.30527753512070888</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1317,23 +1347,23 @@
         <v>703.40769762964896</v>
       </c>
       <c r="L12">
+        <f t="shared" si="2"/>
+        <v>3.6501306297509473E-5</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>3.197231460205785E-5</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>4.2580099732010694</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="3"/>
-        <v>-3.6501306297509473E-5</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>-3.197231460205785E-5</v>
-      </c>
-      <c r="N12" s="4">
-        <f t="shared" si="1"/>
-        <v>4.2580099732010694</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="4"/>
-        <v>1.4193138331933899</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.85">
+        <v>1.4193594822739897</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1365,23 +1395,23 @@
         <v>694.28040598487803</v>
       </c>
       <c r="L13">
+        <f t="shared" si="2"/>
+        <v>2.6828713394877468E-5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>1.534144139725413E-5</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.15064986650099854</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="3"/>
-        <v>-2.6828713394877468E-5</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="0"/>
-        <v>-1.534144139725413E-5</v>
-      </c>
-      <c r="N13" s="4">
-        <f t="shared" si="1"/>
-        <v>0.15064986650099854</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="4"/>
-        <v>5.020256544873547E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.85">
+        <v>5.0230678885263558E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1413,23 +1443,23 @@
         <v>697.30587585965804</v>
       </c>
       <c r="L14">
+        <f t="shared" si="2"/>
+        <v>4.6695832978116414E-6</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>4.2032728799767938E-5</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.20274558779908602</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="3"/>
-        <v>-4.6695832978116414E-6</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
-        <v>-4.2032728799767938E-5</v>
-      </c>
-      <c r="N14" s="4">
-        <f t="shared" si="1"/>
-        <v>-0.20274558779908602</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="4"/>
-        <v>-6.7597430037061201E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.85">
+        <v>6.7597430037061201E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1461,23 +1491,23 @@
         <v>700.40798251111903</v>
       </c>
       <c r="L15">
+        <f t="shared" si="2"/>
+        <v>3.5095372629712074E-4</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>4.0001391270294562E-4</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0.522131438390943</v>
+      </c>
+      <c r="O15">
         <f t="shared" si="3"/>
-        <v>3.5095372629712074E-4</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
-        <v>4.0001391270294562E-4</v>
-      </c>
-      <c r="N15" s="4">
-        <f t="shared" si="1"/>
-        <v>0.522131438390943</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="4"/>
         <v>0.17429413534331437</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1509,23 +1539,23 @@
         <v>691.15933024372998</v>
       </c>
       <c r="L16">
+        <f t="shared" si="2"/>
+        <v>4.370571033973647E-7</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>3.5052682804348478E-5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>3.344619026835062</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="3"/>
-        <v>4.370571033973647E-7</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
-        <v>-3.5052682804348478E-5</v>
-      </c>
-      <c r="N16" s="4">
-        <f t="shared" si="1"/>
-        <v>3.344619026835062</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="4"/>
-        <v>1.1148614704031203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.85">
+        <v>1.1148848388583232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1557,23 +1587,23 @@
         <v>697.04453555616396</v>
       </c>
       <c r="L17">
+        <f t="shared" si="2"/>
+        <v>1.2200819740115776E-4</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>5.1655414601725624E-5</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>2.6865114819470364</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="3"/>
-        <v>1.2200819740115776E-4</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
-        <v>-5.1655414601725624E-5</v>
-      </c>
-      <c r="N17" s="4">
-        <f t="shared" si="1"/>
-        <v>2.6865114819470364</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="4"/>
-        <v>0.8955272782432786</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.85">
+        <v>0.89556171518634642</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1605,23 +1635,23 @@
         <v>696.60393386443695</v>
       </c>
       <c r="L18">
+        <f t="shared" si="2"/>
+        <v>2.3444329890054405E-4</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M32" si="4">ABS(D18-I18)</f>
+        <v>2.3703566209576366E-4</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N32" si="5">ABS(E18-J18)</f>
+        <v>1.0207765895800094</v>
+      </c>
+      <c r="O18">
         <f t="shared" si="3"/>
-        <v>2.3444329890054405E-4</v>
-      </c>
-      <c r="M18">
-        <f>D18-I18</f>
-        <v>2.3703566209576366E-4</v>
-      </c>
-      <c r="N18" s="4">
-        <f t="shared" ref="N18:N32" si="5">E18-J18</f>
-        <v>1.0207765895800094</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="4"/>
         <v>0.3404160228470019</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.85">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1653,23 +1683,23 @@
         <v>704.57555059271499</v>
       </c>
       <c r="L19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.8154140120429929E-4</v>
       </c>
       <c r="M19">
-        <f t="shared" ref="M19:M32" si="6">D19-I19</f>
+        <f t="shared" si="4"/>
         <v>2.3345188979817522E-4</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19">
         <f t="shared" si="5"/>
         <v>1.1032976333970055</v>
       </c>
       <c r="O19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.36790420889600267</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.85">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1701,23 +1731,23 @@
         <v>692.25072441724603</v>
       </c>
       <c r="L20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.2673226795625396E-5</v>
       </c>
       <c r="M20">
-        <f t="shared" si="6"/>
-        <v>-2.6796123300698582E-5</v>
-      </c>
-      <c r="N20" s="4">
+        <f t="shared" si="4"/>
+        <v>2.6796123300698582E-5</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="5"/>
         <v>6.1432416969619226</v>
       </c>
       <c r="O20">
-        <f t="shared" si="4"/>
-        <v>2.047769191355139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.85">
+        <f t="shared" si="3"/>
+        <v>2.0477870554373396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1749,23 +1779,23 @@
         <v>702.71409245966595</v>
       </c>
       <c r="L21">
-        <f t="shared" si="3"/>
-        <v>-1.0563043304046005E-5</v>
+        <f t="shared" si="2"/>
+        <v>1.0563043304046005E-5</v>
       </c>
       <c r="M21">
-        <f t="shared" si="6"/>
-        <v>-3.54525991994592E-5</v>
-      </c>
-      <c r="N21" s="4">
+        <f t="shared" si="4"/>
+        <v>3.54525991994592E-5</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="5"/>
         <v>0.51903750151200256</v>
       </c>
       <c r="O21">
-        <f t="shared" si="4"/>
-        <v>0.1729971619564997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.85">
+        <f t="shared" si="3"/>
+        <v>0.17302783905150201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1797,23 +1827,23 @@
         <v>687.70560595523898</v>
       </c>
       <c r="L22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.4790447509891465E-4</v>
       </c>
       <c r="M22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.9335965330545832E-4</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N22">
         <f t="shared" si="5"/>
         <v>11.282296174121029</v>
       </c>
       <c r="O22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.7609791460831445</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.85">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1845,23 +1875,23 @@
         <v>711.69706157198698</v>
       </c>
       <c r="L23">
+        <f t="shared" si="2"/>
+        <v>3.7846668803354078E-5</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>4.2583563399034574E-5</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>0.28831240708495898</v>
+      </c>
+      <c r="O23">
         <f t="shared" si="3"/>
-        <v>-3.7846668803354078E-5</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="6"/>
-        <v>-4.2583563399034574E-5</v>
-      </c>
-      <c r="N23" s="4">
-        <f t="shared" si="5"/>
-        <v>-0.28831240708495898</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="4"/>
-        <v>-9.6130945772387122E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.85">
+        <v>9.6130945772387122E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1893,23 +1923,23 @@
         <v>693.51150144456403</v>
       </c>
       <c r="L24">
+        <f t="shared" si="2"/>
+        <v>4.6539225340325174E-4</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>4.5312607549874429E-4</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>0.27210878546702588</v>
+      </c>
+      <c r="O24">
         <f t="shared" si="3"/>
-        <v>4.6539225340325174E-4</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="6"/>
-        <v>4.5312607549874429E-4</v>
-      </c>
-      <c r="N24" s="4">
-        <f t="shared" si="5"/>
-        <v>-0.27210878546702588</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="4"/>
-        <v>-9.0396755712707957E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.85">
+        <v>9.1009101265309297E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1941,23 +1971,23 @@
         <v>703.72193385054197</v>
       </c>
       <c r="L25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.4563048059510493E-4</v>
       </c>
       <c r="M25">
-        <f t="shared" si="6"/>
-        <v>-7.5363441901288297E-5</v>
-      </c>
-      <c r="N25" s="4">
+        <f t="shared" si="4"/>
+        <v>7.5363441901288297E-5</v>
+      </c>
+      <c r="N25">
         <f t="shared" si="5"/>
         <v>3.8181115212430541</v>
       </c>
       <c r="O25">
-        <f t="shared" si="4"/>
-        <v>1.2727939294272492</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.85">
+        <f t="shared" si="3"/>
+        <v>1.2728441717218502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1989,23 +2019,23 @@
         <v>690.002706020662</v>
       </c>
       <c r="L26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.2111006380073377E-4</v>
       </c>
       <c r="M26">
-        <f t="shared" si="6"/>
-        <v>-1.6286579189994654E-4</v>
-      </c>
-      <c r="N26" s="4">
+        <f t="shared" si="4"/>
+        <v>1.6286579189994654E-4</v>
+      </c>
+      <c r="N26">
         <f t="shared" si="5"/>
         <v>8.169691405111962</v>
       </c>
       <c r="O26">
-        <f t="shared" si="4"/>
-        <v>2.7233498831279541</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.85">
+        <f t="shared" si="3"/>
+        <v>2.7234584603225542</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2037,23 +2067,23 @@
         <v>701.19780563877703</v>
       </c>
       <c r="L27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8.473771850248113E-5</v>
       </c>
       <c r="M27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3857316210419413E-4</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27">
         <f t="shared" si="5"/>
         <v>3.3397736370500297</v>
       </c>
       <c r="O27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.1133323159768789</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.85">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2085,23 +2115,23 @@
         <v>697.37808696250397</v>
       </c>
       <c r="L28">
+        <f t="shared" si="2"/>
+        <v>5.1924877659814683E-4</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>2.6894257560172719E-4</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>1.1346256592919417</v>
+      </c>
+      <c r="O28">
         <f t="shared" si="3"/>
-        <v>5.1924877659814683E-4</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="6"/>
-        <v>2.6894257560172719E-4</v>
-      </c>
-      <c r="N28" s="4">
-        <f t="shared" si="5"/>
-        <v>-1.1346256592919417</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="4"/>
-        <v>-0.37794582264658061</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.85">
+        <v>0.37847128354804721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2133,23 +2163,23 @@
         <v>693.51766771118105</v>
       </c>
       <c r="L29">
+        <f t="shared" si="2"/>
+        <v>2.791966440440774E-5</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="4"/>
+        <v>1.876883501950033E-6</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>0.16915905088205818</v>
+      </c>
+      <c r="O29">
         <f t="shared" si="3"/>
-        <v>2.791966440440774E-5</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="6"/>
-        <v>1.876883501950033E-6</v>
-      </c>
-      <c r="N29" s="4">
-        <f t="shared" si="5"/>
-        <v>-0.16915905088205818</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="4"/>
-        <v>-5.6376418111383941E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.85">
+        <v>5.6396282476654847E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2181,23 +2211,23 @@
         <v>704.01137275204997</v>
       </c>
       <c r="L30">
-        <f t="shared" si="3"/>
-        <v>-1.7834745099776228E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.7834745099776228E-4</v>
       </c>
       <c r="M30">
-        <f t="shared" si="6"/>
-        <v>-3.7894399198989959E-5</v>
-      </c>
-      <c r="N30" s="4">
+        <f t="shared" si="4"/>
+        <v>3.7894399198989959E-5</v>
+      </c>
+      <c r="N30">
         <f t="shared" si="5"/>
         <v>5.3560998084470839</v>
       </c>
       <c r="O30">
-        <f t="shared" si="4"/>
-        <v>1.7852945221989625</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.85">
+        <f t="shared" si="3"/>
+        <v>1.785438683432427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -2229,23 +2259,23 @@
         <v>696.62096423829405</v>
       </c>
       <c r="L31">
+        <f t="shared" si="2"/>
+        <v>3.4022231403696424E-5</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="4"/>
+        <v>1.4985944919487793E-4</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>3.5124439274241013</v>
+      </c>
+      <c r="O31">
         <f t="shared" si="3"/>
-        <v>3.4022231403696424E-5</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="6"/>
-        <v>1.4985944919487793E-4</v>
-      </c>
-      <c r="N31" s="4">
-        <f t="shared" si="5"/>
-        <v>-3.5124439274241013</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="4"/>
-        <v>-1.1707533485811676</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.85">
+        <v>1.1708759363682333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2277,38 +2307,27 @@
         <v>701.80648950873695</v>
       </c>
       <c r="L32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.4421760699434572E-4</v>
       </c>
       <c r="M32">
-        <f t="shared" si="6"/>
-        <v>-1.6835783740276611E-4</v>
-      </c>
-      <c r="N32" s="4">
+        <f t="shared" si="4"/>
+        <v>1.6835783740276611E-4</v>
+      </c>
+      <c r="N32">
         <f t="shared" si="5"/>
         <v>5.6236994913850822</v>
       </c>
       <c r="O32">
-        <f t="shared" si="4"/>
-        <v>1.8745584503848913</v>
-      </c>
-    </row>
-    <row r="33" spans="5:14" x14ac:dyDescent="0.85">
+        <f t="shared" si="3"/>
+        <v>1.8746706889431597</v>
+      </c>
+    </row>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
-      <c r="L33">
-        <f>AVERAGE(L2:L32)</f>
-        <v>1.2801375275522047E-4</v>
-      </c>
-      <c r="M33">
-        <f>AVERAGE(M2:M32)</f>
-        <v>4.2447077460669716E-5</v>
-      </c>
-      <c r="N33" s="4">
-        <f>AVERAGE(N2:N32)</f>
-        <v>2.5684767965941071</v>
-      </c>
-    </row>
-    <row r="34" spans="5:14" x14ac:dyDescent="0.85">
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
     </row>
   </sheetData>

</xml_diff>